<commit_message>
Introduce and use the CheckPipelineFiles module for the test suite. Finish updating the validation tests.
</commit_message>
<xml_diff>
--- a/tiny/validation/validationUtil/part9_softValidation/MakeFakeExpectations.xlsx
+++ b/tiny/validation/validationUtil/part9_softValidation/MakeFakeExpectations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ieclabau/git/sheepdog_testing_suite/tiny/validation/validationUtil/soft_validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ieclabau/git/sheepdog_testing_suite/tiny/validation/validationUtil/part9_softValidation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5443977B-9F52-F844-9CF7-4E99B5026BA9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BD28AC-2C9C-2841-8D8A-418B3C197D2C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="800" windowWidth="26440" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7160" yWindow="460" windowWidth="26440" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="03_SeqFileValidator_validation" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>name</t>
   </si>
@@ -176,6 +176,60 @@
   </si>
   <si>
     <t>paste values into size column</t>
+  </si>
+  <si>
+    <t>step 1:</t>
+  </si>
+  <si>
+    <t>insert the allowed percentage</t>
+  </si>
+  <si>
+    <t>setp 2:</t>
+  </si>
+  <si>
+    <t>copy all cells from G1 to include all this</t>
+  </si>
+  <si>
+    <t>step 3:</t>
+  </si>
+  <si>
+    <t>paste into G1 in the expectation file</t>
+  </si>
+  <si>
+    <t>step 4:</t>
+  </si>
+  <si>
+    <t>copy value of M column values into column D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">step 5: </t>
+  </si>
+  <si>
+    <t>copy J column values to B</t>
+  </si>
+  <si>
+    <t>step 6:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">step 7: </t>
+  </si>
+  <si>
+    <t>save the modified expectation file</t>
+  </si>
+  <si>
+    <t>step 8:</t>
+  </si>
+  <si>
+    <t>run the test pipeline with stop=N, check output pass/fail against the notes in the expectation file to make sure the new soft validation output is good.</t>
+  </si>
+  <si>
+    <t>save the valiation output as expectation files, and rerun with stop=Y.  If tests pass, you're done.</t>
+  </si>
+  <si>
+    <t>step 9:</t>
+  </si>
+  <si>
+    <t>delete all columns from G to the right</t>
   </si>
 </sst>
 </file>
@@ -318,7 +372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -496,6 +550,30 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -659,15 +737,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1023,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1044,6 +1125,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="6"/>
       <c r="J1" t="s">
         <v>51</v>
       </c>
@@ -1055,39 +1137,39 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>6726</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G2">
         <v>0.01</v>
       </c>
       <c r="H2">
-        <f>B2*G2/100</f>
+        <f t="shared" ref="H2:H22" si="0">B2*G2/100</f>
         <v>0.67260000000000009</v>
       </c>
       <c r="I2">
-        <f>B2+H2</f>
+        <f t="shared" ref="I2:I22" si="1">B2+H2</f>
         <v>6726.6725999999999</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="4">
         <f>ROUND(I2,0)</f>
         <v>6727</v>
       </c>
       <c r="K2">
-        <f>(B2-J2)*100/J2</f>
+        <f t="shared" ref="K2:K22" si="2">(B2-J2)*100/J2</f>
         <v>-1.4865467518953471E-2</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:L22" si="0">IF(ABS(K2)&gt;$L$26,$L$28,$L$27)</f>
+        <f t="shared" ref="L2:L22" si="3">IF(ABS(K2)&gt;$L$26,$L$28,$L$27)</f>
         <v>PASS</v>
       </c>
-      <c r="M2" t="str">
+      <c r="M2" s="3" t="str">
         <f>_xlfn.CONCAT(L2, " - Real value is ", K2, "% different from expectation size.")</f>
         <v>PASS - Real value is -0.0148654675189535% different from expectation size.</v>
       </c>
@@ -1096,40 +1178,40 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>3922</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G3">
         <v>0.1</v>
       </c>
       <c r="H3">
-        <f>B3*G3/100</f>
+        <f t="shared" si="0"/>
         <v>3.9220000000000006</v>
       </c>
       <c r="I3">
-        <f>B3+H3</f>
+        <f t="shared" si="1"/>
         <v>3925.922</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J22" si="1">ROUND(I3,0)</f>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J22" si="4">ROUND(I3,0)</f>
         <v>3926</v>
       </c>
       <c r="K3">
-        <f>(B3-J3)*100/J3</f>
+        <f t="shared" si="2"/>
         <v>-0.10188487009679063</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M3" t="str">
-        <f t="shared" ref="M3:M22" si="2">_xlfn.CONCAT(L3, " - Real value is ", K3, "% different from expectation size.")</f>
+      <c r="M3" s="3" t="str">
+        <f t="shared" ref="M3:M22" si="5">_xlfn.CONCAT(L3, " - Real value is ", K3, "% different from expectation size.")</f>
         <v>PASS - Real value is -0.101884870096791% different from expectation size.</v>
       </c>
     </row>
@@ -1137,40 +1219,40 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>7847</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G4">
         <v>0.5</v>
       </c>
       <c r="H4">
-        <f>B4*G4/100</f>
+        <f t="shared" si="0"/>
         <v>39.234999999999999</v>
       </c>
       <c r="I4">
-        <f>B4+H4</f>
+        <f t="shared" si="1"/>
         <v>7886.2349999999997</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="1"/>
+      <c r="J4" s="4">
+        <f t="shared" si="4"/>
         <v>7886</v>
       </c>
       <c r="K4">
-        <f>(B4-J4)*100/J4</f>
+        <f t="shared" si="2"/>
         <v>-0.49454729901090538</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M4" t="str">
-        <f t="shared" si="2"/>
+      <c r="M4" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is -0.494547299010905% different from expectation size.</v>
       </c>
     </row>
@@ -1178,40 +1260,40 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>831</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G5">
         <v>0.5</v>
       </c>
       <c r="H5">
-        <f>B5*G5/100</f>
+        <f t="shared" si="0"/>
         <v>4.1550000000000002</v>
       </c>
       <c r="I5">
-        <f>B5+H5</f>
+        <f t="shared" si="1"/>
         <v>835.15499999999997</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="1"/>
+      <c r="J5" s="4">
+        <f t="shared" si="4"/>
         <v>835</v>
       </c>
       <c r="K5">
-        <f>(B5-J5)*100/J5</f>
+        <f t="shared" si="2"/>
         <v>-0.47904191616766467</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M5" t="str">
-        <f t="shared" si="2"/>
+      <c r="M5" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is -0.479041916167665% different from expectation size.</v>
       </c>
     </row>
@@ -1219,40 +1301,40 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>5046</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="H6">
-        <f>B6*G6/100</f>
+        <f t="shared" si="0"/>
         <v>100.92</v>
       </c>
       <c r="I6">
-        <f>B6+H6</f>
+        <f t="shared" si="1"/>
         <v>5146.92</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="1"/>
+      <c r="J6" s="4">
+        <f t="shared" si="4"/>
         <v>5147</v>
       </c>
       <c r="K6">
-        <f>(B6-J6)*100/J6</f>
+        <f t="shared" si="2"/>
         <v>-1.9623081406644647</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M6" t="str">
-        <f t="shared" si="2"/>
+      <c r="M6" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is -1.96230814066446% different from expectation size.</v>
       </c>
     </row>
@@ -1260,40 +1342,40 @@
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>4482</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
       <c r="H7">
-        <f>B7*G7/100</f>
+        <f t="shared" si="0"/>
         <v>89.64</v>
       </c>
       <c r="I7">
-        <f>B7+H7</f>
+        <f t="shared" si="1"/>
         <v>4571.6400000000003</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="1"/>
+      <c r="J7" s="4">
+        <f t="shared" si="4"/>
         <v>4572</v>
       </c>
       <c r="K7">
-        <f>(B7-J7)*100/J7</f>
+        <f t="shared" si="2"/>
         <v>-1.9685039370078741</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M7" t="str">
-        <f t="shared" si="2"/>
+      <c r="M7" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is -1.96850393700787% different from expectation size.</v>
       </c>
     </row>
@@ -1301,40 +1383,40 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>2803</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="H8">
-        <f>B8*G8/100</f>
+        <f t="shared" si="0"/>
         <v>56.06</v>
       </c>
       <c r="I8">
-        <f>B8+H8</f>
+        <f t="shared" si="1"/>
         <v>2859.06</v>
       </c>
-      <c r="J8">
-        <f t="shared" si="1"/>
+      <c r="J8" s="4">
+        <f t="shared" si="4"/>
         <v>2859</v>
       </c>
       <c r="K8">
-        <f>(B8-J8)*100/J8</f>
+        <f t="shared" si="2"/>
         <v>-1.9587268275620846</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M8" t="str">
-        <f t="shared" si="2"/>
+      <c r="M8" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is -1.95872682756208% different from expectation size.</v>
       </c>
     </row>
@@ -1342,40 +1424,40 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>2801</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G9">
         <v>5</v>
       </c>
       <c r="H9">
-        <f>B9*G9/100</f>
+        <f t="shared" si="0"/>
         <v>140.05000000000001</v>
       </c>
       <c r="I9">
-        <f>B9+H9</f>
+        <f t="shared" si="1"/>
         <v>2941.05</v>
       </c>
-      <c r="J9">
-        <f t="shared" si="1"/>
+      <c r="J9" s="4">
+        <f t="shared" si="4"/>
         <v>2941</v>
       </c>
       <c r="K9">
-        <f>(B9-J9)*100/J9</f>
+        <f t="shared" si="2"/>
         <v>-4.7602856171370282</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M9" t="str">
-        <f t="shared" si="2"/>
+      <c r="M9" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is -4.76028561713703% different from expectation size.</v>
       </c>
     </row>
@@ -1383,40 +1465,40 @@
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>2802</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G10">
         <v>5</v>
       </c>
       <c r="H10">
-        <f>B10*G10/100</f>
+        <f t="shared" si="0"/>
         <v>140.1</v>
       </c>
       <c r="I10">
-        <f>B10+H10</f>
+        <f t="shared" si="1"/>
         <v>2942.1</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="1"/>
+      <c r="J10" s="4">
+        <f t="shared" si="4"/>
         <v>2942</v>
       </c>
       <c r="K10">
-        <f>(B10-J10)*100/J10</f>
+        <f t="shared" si="2"/>
         <v>-4.7586675730795376</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M10" t="str">
-        <f t="shared" si="2"/>
+      <c r="M10" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is -4.75866757307954% different from expectation size.</v>
       </c>
     </row>
@@ -1424,40 +1506,40 @@
       <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>4484</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G11">
         <v>12</v>
       </c>
       <c r="H11">
-        <f>B11*G11/100</f>
+        <f t="shared" si="0"/>
         <v>538.08000000000004</v>
       </c>
       <c r="I11">
-        <f>B11+H11</f>
+        <f t="shared" si="1"/>
         <v>5022.08</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="1"/>
+      <c r="J11" s="4">
+        <f t="shared" si="4"/>
         <v>5022</v>
       </c>
       <c r="K11">
-        <f>(B11-J11)*100/J11</f>
+        <f t="shared" si="2"/>
         <v>-10.712863401035444</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>FAIL</v>
       </c>
-      <c r="M11" t="str">
-        <f t="shared" si="2"/>
+      <c r="M11" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>FAIL - Real value is -10.7128634010354% different from expectation size.</v>
       </c>
     </row>
@@ -1465,40 +1547,40 @@
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>1120</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G12">
         <v>20</v>
       </c>
       <c r="H12">
-        <f>B12*G12/100</f>
+        <f t="shared" si="0"/>
         <v>224</v>
       </c>
       <c r="I12">
-        <f>B12+H12</f>
-        <v>1344</v>
-      </c>
-      <c r="J12">
         <f t="shared" si="1"/>
         <v>1344</v>
       </c>
+      <c r="J12" s="4">
+        <f t="shared" si="4"/>
+        <v>1344</v>
+      </c>
       <c r="K12">
-        <f>(B12-J12)*100/J12</f>
+        <f t="shared" si="2"/>
         <v>-16.666666666666668</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>FAIL</v>
       </c>
-      <c r="M12" t="str">
-        <f t="shared" si="2"/>
+      <c r="M12" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>FAIL - Real value is -16.6666666666667% different from expectation size.</v>
       </c>
     </row>
@@ -1506,40 +1588,40 @@
       <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>4485</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <f>B13*G13/100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I13">
-        <f>B13+H13</f>
-        <v>4485</v>
-      </c>
-      <c r="J13">
         <f t="shared" si="1"/>
         <v>4485</v>
       </c>
+      <c r="J13" s="4">
+        <f t="shared" si="4"/>
+        <v>4485</v>
+      </c>
       <c r="K13">
-        <f>(B13-J13)*100/J13</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M13" t="str">
-        <f t="shared" si="2"/>
+      <c r="M13" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is 0% different from expectation size.</v>
       </c>
     </row>
@@ -1547,40 +1629,40 @@
       <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <v>1122</v>
       </c>
       <c r="C14" t="s">
         <v>30</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <f>B14*G14/100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I14">
-        <f>B14+H14</f>
-        <v>1122</v>
-      </c>
-      <c r="J14">
         <f t="shared" si="1"/>
         <v>1122</v>
       </c>
+      <c r="J14" s="4">
+        <f t="shared" si="4"/>
+        <v>1122</v>
+      </c>
       <c r="K14">
-        <f>(B14-J14)*100/J14</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M14" t="str">
-        <f t="shared" si="2"/>
+      <c r="M14" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is 0% different from expectation size.</v>
       </c>
     </row>
@@ -1588,40 +1670,40 @@
       <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="4">
         <v>4487</v>
       </c>
       <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G15">
         <v>-0.05</v>
       </c>
       <c r="H15">
-        <f>B15*G15/100</f>
+        <f t="shared" si="0"/>
         <v>-2.2435</v>
       </c>
       <c r="I15">
-        <f>B15+H15</f>
+        <f t="shared" si="1"/>
         <v>4484.7565000000004</v>
       </c>
-      <c r="J15">
-        <f t="shared" si="1"/>
+      <c r="J15" s="4">
+        <f t="shared" si="4"/>
         <v>4485</v>
       </c>
       <c r="K15">
-        <f>(B15-J15)*100/J15</f>
+        <f t="shared" si="2"/>
         <v>4.4593088071348944E-2</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M15" t="str">
-        <f t="shared" si="2"/>
+      <c r="M15" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is 0.0445930880713489% different from expectation size.</v>
       </c>
     </row>
@@ -1629,40 +1711,40 @@
       <c r="A16" t="s">
         <v>33</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>3362</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G16">
         <v>-0.5</v>
       </c>
       <c r="H16">
-        <f>B16*G16/100</f>
+        <f t="shared" si="0"/>
         <v>-16.809999999999999</v>
       </c>
       <c r="I16">
-        <f>B16+H16</f>
+        <f t="shared" si="1"/>
         <v>3345.19</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="1"/>
+      <c r="J16" s="4">
+        <f t="shared" si="4"/>
         <v>3345</v>
       </c>
       <c r="K16">
-        <f>(B16-J16)*100/J16</f>
+        <f t="shared" si="2"/>
         <v>0.50822122571001493</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M16" t="str">
-        <f t="shared" si="2"/>
+      <c r="M16" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is 0.508221225710015% different from expectation size.</v>
       </c>
     </row>
@@ -1670,40 +1752,40 @@
       <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>1683</v>
       </c>
       <c r="C17" t="s">
         <v>36</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G17">
         <v>-2</v>
       </c>
       <c r="H17">
-        <f>B17*G17/100</f>
+        <f t="shared" si="0"/>
         <v>-33.659999999999997</v>
       </c>
       <c r="I17">
-        <f>B17+H17</f>
+        <f t="shared" si="1"/>
         <v>1649.34</v>
       </c>
-      <c r="J17">
-        <f t="shared" si="1"/>
+      <c r="J17" s="4">
+        <f t="shared" si="4"/>
         <v>1649</v>
       </c>
       <c r="K17">
-        <f>(B17-J17)*100/J17</f>
+        <f t="shared" si="2"/>
         <v>2.0618556701030926</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M17" t="str">
-        <f t="shared" si="2"/>
+      <c r="M17" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is 2.06185567010309% different from expectation size.</v>
       </c>
     </row>
@@ -1711,40 +1793,40 @@
       <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <v>5600</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G18">
         <v>-2</v>
       </c>
       <c r="H18">
-        <f>B18*G18/100</f>
+        <f t="shared" si="0"/>
         <v>-112</v>
       </c>
       <c r="I18">
-        <f>B18+H18</f>
-        <v>5488</v>
-      </c>
-      <c r="J18">
         <f t="shared" si="1"/>
         <v>5488</v>
       </c>
+      <c r="J18" s="4">
+        <f t="shared" si="4"/>
+        <v>5488</v>
+      </c>
       <c r="K18">
-        <f>(B18-J18)*100/J18</f>
+        <f t="shared" si="2"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M18" t="str">
-        <f t="shared" si="2"/>
+      <c r="M18" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is 2.04081632653061% different from expectation size.</v>
       </c>
     </row>
@@ -1752,40 +1834,40 @@
       <c r="A19" t="s">
         <v>39</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <v>5607</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G19">
         <v>-2</v>
       </c>
       <c r="H19">
-        <f>B19*G19/100</f>
+        <f t="shared" si="0"/>
         <v>-112.14</v>
       </c>
       <c r="I19">
-        <f>B19+H19</f>
+        <f t="shared" si="1"/>
         <v>5494.86</v>
       </c>
-      <c r="J19">
-        <f t="shared" si="1"/>
+      <c r="J19" s="4">
+        <f t="shared" si="4"/>
         <v>5495</v>
       </c>
       <c r="K19">
-        <f>(B19-J19)*100/J19</f>
+        <f t="shared" si="2"/>
         <v>2.0382165605095541</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>PASS</v>
       </c>
-      <c r="M19" t="str">
-        <f t="shared" si="2"/>
+      <c r="M19" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>PASS - Real value is 2.03821656050955% different from expectation size.</v>
       </c>
     </row>
@@ -1793,40 +1875,40 @@
       <c r="A20" t="s">
         <v>41</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="4">
         <v>7849</v>
       </c>
       <c r="C20" t="s">
         <v>42</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G20">
         <v>-5</v>
       </c>
       <c r="H20">
-        <f>B20*G20/100</f>
+        <f t="shared" si="0"/>
         <v>-392.45</v>
       </c>
       <c r="I20">
-        <f>B20+H20</f>
+        <f t="shared" si="1"/>
         <v>7456.55</v>
       </c>
-      <c r="J20">
-        <f t="shared" si="1"/>
+      <c r="J20" s="4">
+        <f t="shared" si="4"/>
         <v>7457</v>
       </c>
       <c r="K20">
-        <f>(B20-J20)*100/J20</f>
+        <f t="shared" si="2"/>
         <v>5.2568056859326804</v>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>FAIL</v>
       </c>
-      <c r="M20" t="str">
-        <f t="shared" si="2"/>
+      <c r="M20" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>FAIL - Real value is 5.25680568593268% different from expectation size.</v>
       </c>
     </row>
@@ -1834,40 +1916,40 @@
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4">
         <v>6724</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G21">
         <v>-5</v>
       </c>
       <c r="H21">
-        <f>B21*G21/100</f>
+        <f t="shared" si="0"/>
         <v>-336.2</v>
       </c>
       <c r="I21">
-        <f>B21+H21</f>
+        <f t="shared" si="1"/>
         <v>6387.8</v>
       </c>
-      <c r="J21">
-        <f t="shared" si="1"/>
+      <c r="J21" s="4">
+        <f t="shared" si="4"/>
         <v>6388</v>
       </c>
       <c r="K21">
-        <f>(B21-J21)*100/J21</f>
+        <f t="shared" si="2"/>
         <v>5.2598622417031935</v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>FAIL</v>
       </c>
-      <c r="M21" t="str">
-        <f t="shared" si="2"/>
+      <c r="M21" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>FAIL - Real value is 5.25986224170319% different from expectation size.</v>
       </c>
     </row>
@@ -1875,60 +1957,126 @@
       <c r="A22" t="s">
         <v>45</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="4">
         <v>4484</v>
       </c>
       <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G22">
         <v>-12</v>
       </c>
       <c r="H22">
-        <f>B22*G22/100</f>
+        <f t="shared" si="0"/>
         <v>-538.08000000000004</v>
       </c>
       <c r="I22">
-        <f>B22+H22</f>
+        <f t="shared" si="1"/>
         <v>3945.92</v>
       </c>
-      <c r="J22">
-        <f t="shared" si="1"/>
+      <c r="J22" s="4">
+        <f t="shared" si="4"/>
         <v>3946</v>
       </c>
       <c r="K22">
-        <f>(B22-J22)*100/J22</f>
+        <f t="shared" si="2"/>
         <v>13.634059807399899</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>FAIL</v>
       </c>
-      <c r="M22" t="str">
-        <f t="shared" si="2"/>
+      <c r="M22" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>FAIL - Real value is 13.6340598073999% different from expectation size.</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" t="s">
+        <v>53</v>
+      </c>
       <c r="K26" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L26" s="3">
+      <c r="L26" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" t="s">
+        <v>55</v>
+      </c>
       <c r="K27" s="2"/>
       <c r="L27" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" t="s">
+        <v>57</v>
+      </c>
       <c r="L28" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>62</v>
+      </c>
+      <c r="H31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>63</v>
+      </c>
+      <c r="H32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>65</v>
+      </c>
+      <c r="H33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>